<commit_message>
day 18 2021 now parsing
</commit_message>
<xml_diff>
--- a/Day18/workings.xlsx
+++ b/Day18/workings.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2705B56-B03E-9D4F-B4FC-096ABE596A0E}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33660FFE-84BF-644E-910A-8C0CF5C7FF05}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="arrays" sheetId="1" r:id="rId1"/>
+    <sheet name="parsing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>[[[[[9,8],1],2],3],4]</t>
   </si>
@@ -75,6 +76,15 @@
     <t>,4]</t>
   </si>
   <si>
+    <t>[[</t>
+  </si>
+  <si>
+    <t>[[[</t>
+  </si>
+  <si>
+    <t>[[[[</t>
+  </si>
+  <si>
     <t>[7,[6,[5,[4,[3,2]]]]]</t>
   </si>
   <si>
@@ -138,13 +148,40 @@
     <t>[[6,[5,[4,</t>
   </si>
   <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>[9,8],1],2],3],4]</t>
+  </si>
+  <si>
+    <t>[[9,8],1],2],3],4]</t>
+  </si>
+  <si>
+    <t>[[[9,8],1],2],3],4]</t>
+  </si>
+  <si>
+    <t>[[[[9,8],1],2],3],4]</t>
+  </si>
+  <si>
     <t>,3]</t>
   </si>
   <si>
     <t>,2]</t>
   </si>
   <si>
-    <t>^</t>
+    <t>stack</t>
+  </si>
+  <si>
+    <t>[[[[[</t>
+  </si>
+  <si>
+    <t>9,8],1],2],3],4]</t>
+  </si>
+  <si>
+    <t>explode</t>
+  </si>
+  <si>
+    <t>0,     9],2],3],4]</t>
   </si>
 </sst>
 </file>
@@ -180,10 +217,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,7 +542,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,7 +600,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -577,13 +617,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -594,13 +634,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -611,13 +651,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -625,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -633,16 +673,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -650,16 +690,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -667,16 +707,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -684,16 +724,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -701,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -712,13 +752,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -726,16 +766,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -743,16 +783,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -760,16 +800,214 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C842AC0-9B2A-8C46-AFD7-DA40DCA8015C}">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3</v>
+      </c>
+      <c r="H19" s="2">
+        <v>4</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>3</v>
+      </c>
+      <c r="J20" s="2">
+        <v>4</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 18 2021 parse works
</commit_message>
<xml_diff>
--- a/Day18/workings.xlsx
+++ b/Day18/workings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="222" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33660FFE-84BF-644E-910A-8C0CF5C7FF05}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F81C7400-74CA-374A-8485-18D540D3CC04}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="1" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
   </bookViews>
   <sheets>
     <sheet name="arrays" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
   <si>
     <t>[[[[[9,8],1],2],3],4]</t>
   </si>
@@ -76,12 +76,6 @@
     <t>,4]</t>
   </si>
   <si>
-    <t>[[</t>
-  </si>
-  <si>
-    <t>[[[</t>
-  </si>
-  <si>
     <t>[[[[</t>
   </si>
   <si>
@@ -148,40 +142,40 @@
     <t>[[6,[5,[4,</t>
   </si>
   <si>
-    <t>str</t>
-  </si>
-  <si>
-    <t>[9,8],1],2],3],4]</t>
-  </si>
-  <si>
-    <t>[[9,8],1],2],3],4]</t>
-  </si>
-  <si>
-    <t>[[[9,8],1],2],3],4]</t>
-  </si>
-  <si>
-    <t>[[[[9,8],1],2],3],4]</t>
-  </si>
-  <si>
     <t>,3]</t>
   </si>
   <si>
     <t>,2]</t>
   </si>
   <si>
-    <t>stack</t>
-  </si>
-  <si>
-    <t>[[[[[</t>
-  </si>
-  <si>
-    <t>9,8],1],2],3],4]</t>
-  </si>
-  <si>
-    <t>explode</t>
-  </si>
-  <si>
-    <t>0,     9],2],3],4]</t>
+    <t>updateLeft</t>
+  </si>
+  <si>
+    <t>updateRight</t>
+  </si>
+  <si>
+    <t>,9],2],3],4]</t>
+  </si>
+  <si>
+    <t>[[[0,9],2],3],4]</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>ch</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>[[[[0,7],4],[15,[0,13]]],[1,1]]</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -217,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +219,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D030818D-AB5A-2E4A-A636-E84938471C28}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -623,7 +621,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -640,7 +638,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -657,7 +655,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -665,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -673,16 +671,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -690,16 +688,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -707,16 +705,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -724,16 +722,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -741,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -752,13 +750,13 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -766,16 +764,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -783,16 +781,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -800,16 +798,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -819,195 +817,199 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C842AC0-9B2A-8C46-AFD7-DA40DCA8015C}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="11" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="2.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2">
-        <v>4</v>
-      </c>
-      <c r="E17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2">
-        <v>3</v>
-      </c>
-      <c r="F18" s="2">
-        <v>4</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2</v>
-      </c>
-      <c r="G19" s="2">
-        <v>3</v>
-      </c>
-      <c r="H19" s="2">
-        <v>4</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2">
-        <v>2</v>
-      </c>
-      <c r="I20" s="2">
-        <v>3</v>
-      </c>
-      <c r="J20" s="2">
-        <v>4</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>19</v>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 18 2021 explode not priority
</commit_message>
<xml_diff>
--- a/Day18/workings.xlsx
+++ b/Day18/workings.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{695AFE37-DFDB-2246-8908-4CF67D0F7879}"/>
+  <xr:revisionPtr revIDLastSave="486" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99E7B251-543D-E043-AB86-8F1C1FDCF83E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="1" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="3" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
   </bookViews>
   <sheets>
     <sheet name="arrays" sheetId="1" r:id="rId1"/>
     <sheet name="parsing" sheetId="2" r:id="rId2"/>
+    <sheet name="example 4" sheetId="3" r:id="rId3"/>
+    <sheet name="example 4 (2)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>[[[[[9,8],1],2],3],4]</t>
   </si>
@@ -155,13 +157,688 @@
   </si>
   <si>
     <t>[[[[0,7],4],[[17,8],[0,13]]],[1,1]]</t>
+  </si>
+  <si>
+    <r>
+      <t>[[[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[4,5]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[0,0]],[[[4,5],[2,6]],[9,5]]],[7,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,0]],[[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[4,5]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[2,6]],[9,5]]],[7,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[7,6]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[9,5]]],[7,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,5]]],[7,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[7,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,5]]],[7,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]],[7,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]],[7,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[[[3,7],[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[7,7],[[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[3,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[7,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[[0,[11,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[7,[5,5]],[[0,[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[7,[5,5]],[[0,[[5,6],3]],[[6,3],[8,8]]]]]</t>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[7,[5,5]],[[0,[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[5,6]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <t>explode</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[7,[[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[3,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[4,3]],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[11,3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[11,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[9,3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[11,9],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[11,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,5]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[7,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,5]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,9],[[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,9],[[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[5,6]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[[0,15],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[7,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[9,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]]]</t>
+    </r>
+  </si>
+  <si>
+    <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[5,0]]]]</t>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[5,5]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]]]</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +852,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Source Code Pro"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Source Code Pro"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,6 +931,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,7 +1528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C842AC0-9B2A-8C46-AFD7-DA40DCA8015C}">
   <dimension ref="D2:AN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -1070,139 +1759,139 @@
         <v>38</v>
       </c>
       <c r="E4" s="3" t="str">
-        <f>MID($D$4,E2,1)</f>
+        <f t="shared" ref="E4:AL4" si="0">MID($D$4,E2,1)</f>
         <v>[</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>MID($D$4,F2,1)</f>
+        <f t="shared" si="0"/>
         <v>[</v>
       </c>
       <c r="G4" s="3" t="str">
-        <f>MID($D$4,G2,1)</f>
+        <f t="shared" si="0"/>
         <v>[</v>
       </c>
       <c r="H4" s="3" t="str">
-        <f>MID($D$4,H2,1)</f>
+        <f t="shared" si="0"/>
         <v>[</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f>MID($D$4,I2,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="3" t="str">
-        <f>MID($D$4,J2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="K4" s="3" t="str">
-        <f>MID($D$4,K2,1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L4" s="3" t="str">
-        <f>MID($D$4,L2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
       <c r="M4" s="3" t="str">
-        <f>MID($D$4,M2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="N4" s="3" t="str">
-        <f>MID($D$4,N2,1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="O4" s="3" t="str">
-        <f>MID($D$4,O2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
       <c r="P4" s="3" t="str">
-        <f>MID($D$4,P2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="Q4" s="3" t="str">
-        <f>MID($D$4,Q2,1)</f>
+        <f t="shared" si="0"/>
         <v>[</v>
       </c>
       <c r="R4" s="3" t="str">
-        <f>MID($D$4,R2,1)</f>
+        <f t="shared" si="0"/>
         <v>[</v>
       </c>
       <c r="S4" s="3" t="str">
-        <f>MID($D$4,S2,1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="T4" s="3" t="str">
-        <f>MID($D$4,T2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="U4" s="3" t="str">
-        <f>MID($D$4,U2,1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="V4" s="3" t="str">
-        <f>MID($D$4,V2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
       <c r="W4" s="3" t="str">
-        <f>MID($D$4,W2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="X4" s="3" t="str">
-        <f>MID($D$4,X2,1)</f>
+        <f t="shared" si="0"/>
         <v>[</v>
       </c>
       <c r="Y4" s="3" t="str">
-        <f>MID($D$4,Y2,1)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Z4" s="3" t="str">
-        <f>MID($D$4,Z2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="AA4" s="3" t="str">
-        <f>MID($D$4,AA2,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AB4" s="3" t="str">
-        <f>MID($D$4,AB2,1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AC4" s="3" t="str">
-        <f>MID($D$4,AC2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
       <c r="AD4" s="3" t="str">
-        <f>MID($D$4,AD2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
       <c r="AE4" s="3" t="str">
-        <f>MID($D$4,AE2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
       <c r="AF4" s="3" t="str">
-        <f>MID($D$4,AF2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="AG4" s="3" t="str">
-        <f>MID($D$4,AG2,1)</f>
+        <f t="shared" si="0"/>
         <v>[</v>
       </c>
       <c r="AH4" s="3" t="str">
-        <f>MID($D$4,AH2,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AI4" s="3" t="str">
-        <f>MID($D$4,AI2,1)</f>
+        <f t="shared" si="0"/>
         <v>,</v>
       </c>
       <c r="AJ4" s="3" t="str">
-        <f>MID($D$4,AJ2,1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AK4" s="3" t="str">
-        <f>MID($D$4,AK2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
       <c r="AL4" s="3" t="str">
-        <f>MID($D$4,AL2,1)</f>
+        <f t="shared" si="0"/>
         <v>]</v>
       </c>
     </row>
@@ -1423,135 +2112,135 @@
         <v>[</v>
       </c>
       <c r="F8" s="3" t="str">
-        <f t="shared" ref="F8:AL8" si="0">MID($D$8,F6,1)</f>
+        <f t="shared" ref="F8:AL8" si="1">MID($D$8,F6,1)</f>
         <v>[</v>
       </c>
       <c r="G8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[</v>
       </c>
       <c r="H8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[</v>
       </c>
       <c r="I8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,</v>
       </c>
       <c r="K8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>]</v>
       </c>
       <c r="M8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,</v>
       </c>
       <c r="N8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="O8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>]</v>
       </c>
       <c r="P8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,</v>
       </c>
       <c r="Q8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[</v>
       </c>
       <c r="R8" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S8" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="T8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,</v>
       </c>
       <c r="U8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[</v>
       </c>
       <c r="V8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,</v>
       </c>
       <c r="X8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Y8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Z8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>]</v>
       </c>
       <c r="AA8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>]</v>
       </c>
       <c r="AB8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>]</v>
       </c>
       <c r="AC8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,</v>
       </c>
       <c r="AD8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>[</v>
       </c>
       <c r="AE8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AF8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>,</v>
       </c>
       <c r="AG8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AH8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>]</v>
       </c>
       <c r="AI8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>]</v>
       </c>
       <c r="AJ8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AK8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="AL8" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -1784,143 +2473,143 @@
         <v>[</v>
       </c>
       <c r="F12" s="3" t="str">
-        <f t="shared" ref="F12:AL12" si="1">MID($D$12,F10,1)</f>
+        <f t="shared" ref="F12:AL12" si="2">MID($D$12,F10,1)</f>
         <v>[</v>
       </c>
       <c r="G12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[</v>
       </c>
       <c r="H12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[</v>
       </c>
       <c r="I12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="K12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>]</v>
       </c>
       <c r="M12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="N12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>]</v>
       </c>
       <c r="P12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="Q12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[</v>
       </c>
       <c r="R12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[</v>
       </c>
       <c r="S12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="T12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="U12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="V12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="W12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>]</v>
       </c>
       <c r="X12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="Y12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[</v>
       </c>
       <c r="Z12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA12" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="AB12" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AC12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AD12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>]</v>
       </c>
       <c r="AE12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>]</v>
       </c>
       <c r="AF12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>]</v>
       </c>
       <c r="AG12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="AH12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[</v>
       </c>
       <c r="AI12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AJ12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>,</v>
       </c>
       <c r="AK12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AL12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>]</v>
       </c>
       <c r="AM12" s="3" t="str">
-        <f t="shared" ref="AM12:AN12" si="2">MID($D$12,AM10,1)</f>
+        <f t="shared" ref="AM12:AN12" si="3">MID($D$12,AM10,1)</f>
         <v>]</v>
       </c>
       <c r="AN12" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2141,135 +2830,135 @@
         <v>[</v>
       </c>
       <c r="F16" s="3" t="str">
-        <f t="shared" ref="F16:AL16" si="3">MID($D$12,F14,1)</f>
+        <f t="shared" ref="F16:AL16" si="4">MID($D$12,F14,1)</f>
         <v>[</v>
       </c>
       <c r="G16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
       <c r="H16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
       <c r="I16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="K16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
       <c r="M16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="N16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="O16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
       <c r="P16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="Q16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
       <c r="R16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
       <c r="S16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="U16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="V16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="W16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
       <c r="X16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="Y16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
       <c r="Z16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AA16" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="AB16" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AC16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AD16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
       <c r="AE16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
       <c r="AF16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
       <c r="AG16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="AH16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>[</v>
       </c>
       <c r="AI16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AJ16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>,</v>
       </c>
       <c r="AK16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AL16" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>]</v>
       </c>
     </row>
@@ -2490,136 +3179,449 @@
         <v>[</v>
       </c>
       <c r="F20" s="3" t="str">
-        <f t="shared" ref="F20:AL20" si="4">MID($D$12,F18,1)</f>
+        <f t="shared" ref="F20:AL20" si="5">MID($D$12,F18,1)</f>
         <v>[</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>[</v>
       </c>
       <c r="H20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>[</v>
       </c>
       <c r="I20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="K20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
       </c>
       <c r="M20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="N20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="O20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
       </c>
       <c r="P20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="Q20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>[</v>
       </c>
       <c r="R20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>[</v>
       </c>
       <c r="S20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="T20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="U20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="V20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="W20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
       </c>
       <c r="X20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="Y20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>[</v>
       </c>
       <c r="Z20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA20" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="AB20" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AC20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="AD20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
       </c>
       <c r="AE20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
       </c>
       <c r="AF20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
       </c>
       <c r="AG20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="AH20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>[</v>
       </c>
       <c r="AI20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AJ20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>,</v>
       </c>
       <c r="AK20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="AL20" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9531698A-1CAE-1D4F-9D89-245E96E7BEE7}">
+  <dimension ref="A2:B14"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="147" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FCBDEB-4D47-AB41-A005-324F5A14173A}">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="147" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 18 2021 works up to example 7
</commit_message>
<xml_diff>
--- a/Day18/workings.xlsx
+++ b/Day18/workings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99E7B251-543D-E043-AB86-8F1C1FDCF83E}"/>
+  <xr:revisionPtr revIDLastSave="487" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4026C497-AB65-804D-9986-897868CC091A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="3" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
   </bookViews>
@@ -433,13 +433,393 @@
   </si>
   <si>
     <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[11,3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[[6,3],[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[11,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[9,3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[8,8]]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[11,9],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[11,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,5]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[7,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,5]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[6,7]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]],[10,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,[[11,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,9],[[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,9],[[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[5,6]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,9],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[[0,15],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[7,8]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>],[11,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,0],[</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[9,10]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>,0]]]]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]]]</t>
+    </r>
+  </si>
+  <si>
+    <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[5,0]]]]</t>
+  </si>
+  <si>
+    <r>
+      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>[5,5]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Source Code Pro"/>
+      </rPr>
+      <t>]]]]</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
       <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[7,[[</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="18"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Source Code Pro"/>
       </rPr>
       <t>[3,7]</t>
@@ -447,398 +827,18 @@
     <r>
       <rPr>
         <sz val="18"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Source Code Pro"/>
       </rPr>
       <t>,[4,3]],[[6,3],[8,8]]]]]</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[11,3]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>],[[6,3],[8,8]]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[11,0],[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[9,3]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,[8,8]]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,0],[15,5]]],[10,[[11,9],[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[11,8]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,0],[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,5]]],[10,[[11,9],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,0],[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[7,8]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,5]]],[10,[[11,9],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>]]],[10,[[11,9],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[6,7]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>]]],[10,[[11,9],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>17</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,[[11,9],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,9],[[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,9],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,9],[[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[5,6]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,9],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>],[[0,15],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[7,8]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>],[11,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,0],[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>19</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,0],[</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[9,10]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>,0]]]]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>]]]]</t>
-    </r>
-  </si>
-  <si>
-    <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[5,0]]]]</t>
-  </si>
-  <si>
-    <r>
-      <t>[[[[4,0],[5,4]],[[7,7],[6,0]]],[[8,[7,7]],[[7,9],[0,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>[5,5]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Source Code Pro"/>
-      </rPr>
-      <t>]]]]</t>
-    </r>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -862,6 +862,17 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Source Code Pro"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Source Code Pro"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
       <name val="Source Code Pro"/>
     </font>
   </fonts>
@@ -911,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -932,6 +943,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3440,7 +3452,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0.3"/>
@@ -3476,8 +3488,8 @@
       <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>55</v>
+      <c r="B4" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -3485,7 +3497,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -3493,7 +3505,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -3501,7 +3513,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3509,7 +3521,7 @@
         <v>54</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -3517,7 +3529,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -3525,7 +3537,7 @@
         <v>54</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -3533,7 +3545,7 @@
         <v>53</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -3541,7 +3553,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -3549,7 +3561,7 @@
         <v>54</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -3557,7 +3569,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -3565,7 +3577,7 @@
         <v>54</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -3573,7 +3585,7 @@
         <v>54</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3581,7 +3593,7 @@
         <v>53</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3589,7 +3601,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3597,7 +3609,7 @@
         <v>53</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3605,7 +3617,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3613,15 +3625,15 @@
         <v>53</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
day 18 2021 Done!
</commit_message>
<xml_diff>
--- a/Day18/workings.xlsx
+++ b/Day18/workings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1335" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51DF4B3E-EC63-0D46-85FA-9EC41A9F1450}"/>
+  <xr:revisionPtr revIDLastSave="1337" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F535C15E-D922-2242-912D-A063FC93D5F2}"/>
   <bookViews>
-    <workbookView xWindow="16960" yWindow="-21100" windowWidth="38380" windowHeight="21100" activeTab="4" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
+    <workbookView xWindow="-21460" yWindow="-21100" windowWidth="38380" windowHeight="21100" activeTab="4" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
   </bookViews>
   <sheets>
     <sheet name="arrays" sheetId="1" r:id="rId1"/>
@@ -4132,8 +4132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57ECC8A-E00B-B243-9A5B-6ABCEC2F4C1C}">
   <dimension ref="A1:BP100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -4484,7 +4484,7 @@
         <v>,</v>
       </c>
       <c r="AJ2" s="21" t="str">
-        <f t="shared" ref="AJ2:BO2" si="1">MID($C$2,AJ1,1)</f>
+        <f t="shared" ref="AJ2:BC2" si="1">MID($C$2,AJ1,1)</f>
         <v>[</v>
       </c>
       <c r="AK2" s="21" t="str">
@@ -4618,7 +4618,7 @@
     </row>
     <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
-        <f t="shared" ref="A3:A18" si="3">LEN(C3)</f>
+        <f t="shared" ref="A3:A9" si="3">LEN(C3)</f>
         <v>62</v>
       </c>
       <c r="B3" s="19" cm="1">
@@ -19629,7 +19629,7 @@
     </row>
     <row r="77" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A77" s="20">
-        <f t="shared" ref="A77:A100" si="129">LEN(C77)</f>
+        <f t="shared" ref="A77:A97" si="129">LEN(C77)</f>
         <v>43</v>
       </c>
       <c r="B77" s="19" cm="1">

</xml_diff>

<commit_message>
day 19 - 24 transforms?
</commit_message>
<xml_diff>
--- a/Day18/workings.xlsx
+++ b/Day18/workings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tesco-my.sharepoint.com/personal/craig_roberts_tesco_com/Documents/Dev/AdventOfCode/2021/day18/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1337" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F535C15E-D922-2242-912D-A063FC93D5F2}"/>
+  <xr:revisionPtr revIDLastSave="1341" documentId="8_{757A4133-0879-A54E-98F9-AF626AA30B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E750EF-E077-9049-B821-325DFD94622B}"/>
   <bookViews>
-    <workbookView xWindow="-21460" yWindow="-21100" windowWidth="38380" windowHeight="21100" activeTab="4" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
+    <workbookView xWindow="17080" yWindow="-21100" windowWidth="20840" windowHeight="19460" activeTab="4" xr2:uid="{36414A1D-0B69-AB4C-AE32-8BB3AC3D464D}"/>
   </bookViews>
   <sheets>
     <sheet name="arrays" sheetId="1" r:id="rId1"/>
@@ -1020,12 +1020,6 @@
     <t>[[[[13,0],[7,6]],[[5,10],[13,17]]],[3,9]]</t>
   </si>
   <si>
-    <t>[[[[[6,6],0],[7,6]],[[5,10],[13,17]]],[3,9]]</t>
-  </si>
-  <si>
-    <t>[[[[0,6],[7,6]],[[5,10],[13,17]]],[3,9]]</t>
-  </si>
-  <si>
     <t>[[[[0,6],[7,6]],[[5,[5,5]],[13,17]]],[3,9]]</t>
   </si>
   <si>
@@ -1145,12 +1139,18 @@
   <si>
     <t>[[[[6,6],[6,7]],[[0,7],[7,7]]],[[[5,5],[5,6]],9]]</t>
   </si>
+  <si>
+    <t>[[[[[6,7],0],[7,6]],[[5,10],[13,17]]],[3,9]]</t>
+  </si>
+  <si>
+    <t>[[[[0,7],[7,6]],[[5,10],[13,17]]],[3,9]]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1258,13 +1258,6 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1409,16 +1402,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1428,6 +1418,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4132,8 +4125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57ECC8A-E00B-B243-9A5B-6ABCEC2F4C1C}">
   <dimension ref="A1:BP100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57:K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -4146,200 +4139,200 @@
     <col min="69" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="26" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="D1" s="26">
+    <row r="1" spans="1:68" s="25" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="D1" s="25">
         <v>1</v>
       </c>
-      <c r="E1" s="26">
+      <c r="E1" s="25">
         <v>2</v>
       </c>
-      <c r="F1" s="26">
+      <c r="F1" s="25">
         <v>3</v>
       </c>
-      <c r="G1" s="26">
+      <c r="G1" s="25">
         <v>4</v>
       </c>
-      <c r="H1" s="26">
+      <c r="H1" s="25">
         <v>5</v>
       </c>
-      <c r="I1" s="26">
+      <c r="I1" s="25">
         <v>6</v>
       </c>
-      <c r="J1" s="26">
+      <c r="J1" s="25">
         <v>7</v>
       </c>
-      <c r="K1" s="26">
+      <c r="K1" s="25">
         <v>8</v>
       </c>
-      <c r="L1" s="26">
+      <c r="L1" s="25">
         <v>9</v>
       </c>
-      <c r="M1" s="26">
+      <c r="M1" s="25">
         <v>10</v>
       </c>
-      <c r="N1" s="26">
+      <c r="N1" s="25">
         <v>11</v>
       </c>
-      <c r="O1" s="26">
+      <c r="O1" s="25">
         <v>12</v>
       </c>
-      <c r="P1" s="26">
+      <c r="P1" s="25">
         <v>13</v>
       </c>
-      <c r="Q1" s="26">
+      <c r="Q1" s="25">
         <v>14</v>
       </c>
-      <c r="R1" s="26">
+      <c r="R1" s="25">
         <v>15</v>
       </c>
-      <c r="S1" s="26">
+      <c r="S1" s="25">
         <v>16</v>
       </c>
-      <c r="T1" s="26">
+      <c r="T1" s="25">
         <v>17</v>
       </c>
-      <c r="U1" s="26">
+      <c r="U1" s="25">
         <v>18</v>
       </c>
-      <c r="V1" s="26">
+      <c r="V1" s="25">
         <v>19</v>
       </c>
-      <c r="W1" s="26">
+      <c r="W1" s="25">
         <v>20</v>
       </c>
-      <c r="X1" s="26">
+      <c r="X1" s="25">
         <v>21</v>
       </c>
-      <c r="Y1" s="26">
+      <c r="Y1" s="25">
         <v>22</v>
       </c>
-      <c r="Z1" s="26">
+      <c r="Z1" s="25">
         <v>23</v>
       </c>
-      <c r="AA1" s="26">
+      <c r="AA1" s="25">
         <v>24</v>
       </c>
-      <c r="AB1" s="26">
+      <c r="AB1" s="25">
         <v>25</v>
       </c>
-      <c r="AC1" s="26">
+      <c r="AC1" s="25">
         <v>26</v>
       </c>
-      <c r="AD1" s="26">
+      <c r="AD1" s="25">
         <v>27</v>
       </c>
-      <c r="AE1" s="26">
+      <c r="AE1" s="25">
         <v>28</v>
       </c>
-      <c r="AF1" s="26">
+      <c r="AF1" s="25">
         <v>29</v>
       </c>
-      <c r="AG1" s="26">
+      <c r="AG1" s="25">
         <v>30</v>
       </c>
-      <c r="AH1" s="26">
+      <c r="AH1" s="25">
         <v>31</v>
       </c>
-      <c r="AI1" s="26">
+      <c r="AI1" s="25">
         <v>32</v>
       </c>
-      <c r="AJ1" s="26">
+      <c r="AJ1" s="25">
         <v>33</v>
       </c>
-      <c r="AK1" s="26">
+      <c r="AK1" s="25">
         <v>34</v>
       </c>
-      <c r="AL1" s="26">
+      <c r="AL1" s="25">
         <v>35</v>
       </c>
-      <c r="AM1" s="26">
+      <c r="AM1" s="25">
         <v>36</v>
       </c>
-      <c r="AN1" s="26">
+      <c r="AN1" s="25">
         <v>37</v>
       </c>
-      <c r="AO1" s="26">
+      <c r="AO1" s="25">
         <v>38</v>
       </c>
-      <c r="AP1" s="26">
+      <c r="AP1" s="25">
         <v>39</v>
       </c>
-      <c r="AQ1" s="26">
+      <c r="AQ1" s="25">
         <v>40</v>
       </c>
-      <c r="AR1" s="26">
+      <c r="AR1" s="25">
         <v>41</v>
       </c>
-      <c r="AS1" s="26">
+      <c r="AS1" s="25">
         <v>42</v>
       </c>
-      <c r="AT1" s="26">
+      <c r="AT1" s="25">
         <v>43</v>
       </c>
-      <c r="AU1" s="26">
+      <c r="AU1" s="25">
         <v>44</v>
       </c>
-      <c r="AV1" s="26">
+      <c r="AV1" s="25">
         <v>45</v>
       </c>
-      <c r="AW1" s="26">
+      <c r="AW1" s="25">
         <v>46</v>
       </c>
-      <c r="AX1" s="26">
+      <c r="AX1" s="25">
         <v>47</v>
       </c>
-      <c r="AY1" s="26">
+      <c r="AY1" s="25">
         <v>48</v>
       </c>
-      <c r="AZ1" s="26">
+      <c r="AZ1" s="25">
         <v>49</v>
       </c>
-      <c r="BA1" s="26">
+      <c r="BA1" s="25">
         <v>50</v>
       </c>
-      <c r="BB1" s="26">
+      <c r="BB1" s="25">
         <v>51</v>
       </c>
-      <c r="BC1" s="26">
+      <c r="BC1" s="25">
         <v>52</v>
       </c>
-      <c r="BD1" s="26">
+      <c r="BD1" s="25">
         <v>53</v>
       </c>
-      <c r="BE1" s="26">
+      <c r="BE1" s="25">
         <v>54</v>
       </c>
-      <c r="BF1" s="26">
+      <c r="BF1" s="25">
         <v>55</v>
       </c>
-      <c r="BG1" s="26">
+      <c r="BG1" s="25">
         <v>56</v>
       </c>
-      <c r="BH1" s="26">
+      <c r="BH1" s="25">
         <v>57</v>
       </c>
-      <c r="BI1" s="26">
+      <c r="BI1" s="25">
         <v>58</v>
       </c>
-      <c r="BJ1" s="26">
+      <c r="BJ1" s="25">
         <v>59</v>
       </c>
-      <c r="BK1" s="26">
+      <c r="BK1" s="25">
         <v>60</v>
       </c>
-      <c r="BL1" s="26">
+      <c r="BL1" s="25">
         <v>61</v>
       </c>
-      <c r="BM1" s="26">
+      <c r="BM1" s="25">
         <v>62</v>
       </c>
-      <c r="BN1" s="26">
+      <c r="BN1" s="25">
         <v>63</v>
       </c>
-      <c r="BO1" s="26">
+      <c r="BO1" s="25">
         <v>64</v>
       </c>
-      <c r="BP1" s="26">
+      <c r="BP1" s="25">
         <v>65</v>
       </c>
     </row>
@@ -6063,7 +6056,7 @@
         <f t="array" ref="B9">SUM(LEN(D9:DP9)-LEN(SUBSTITUTE(D9:DP9,"[","")))-SUM(LEN(D9:DP9)-LEN(SUBSTITUTE(D9:DP9,"]","")))</f>
         <v>0</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="20" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="21" t="str">
@@ -7493,31 +7486,31 @@
         <f t="shared" si="28"/>
         <v>,</v>
       </c>
-      <c r="P16" s="25" t="str">
+      <c r="P16" s="24" t="str">
         <f t="shared" si="28"/>
         <v>[</v>
       </c>
-      <c r="Q16" s="25" t="str">
+      <c r="Q16" s="24" t="str">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="R16" s="25" t="str">
+      <c r="R16" s="24" t="str">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="S16" s="25" t="str">
+      <c r="S16" s="24" t="str">
         <f t="shared" si="28"/>
         <v>,</v>
       </c>
-      <c r="T16" s="25" t="str">
+      <c r="T16" s="24" t="str">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="U16" s="25" t="str">
+      <c r="U16" s="24" t="str">
         <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="V16" s="25" t="str">
+      <c r="V16" s="24" t="str">
         <f t="shared" si="28"/>
         <v>]</v>
       </c>
@@ -7686,11 +7679,11 @@
         <f t="shared" si="30"/>
         <v>[</v>
       </c>
-      <c r="N17" s="25" t="str">
+      <c r="N17" s="24" t="str">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
-      <c r="O17" s="25" t="str">
+      <c r="O17" s="24" t="str">
         <f t="shared" si="30"/>
         <v>1</v>
       </c>
@@ -7879,23 +7872,23 @@
         <f t="shared" si="31"/>
         <v>[</v>
       </c>
-      <c r="N18" s="25" t="str">
+      <c r="N18" s="24" t="str">
         <f t="shared" si="31"/>
         <v>[</v>
       </c>
-      <c r="O18" s="25" t="str">
+      <c r="O18" s="24" t="str">
         <f t="shared" si="31"/>
         <v>5</v>
       </c>
-      <c r="P18" s="25" t="str">
+      <c r="P18" s="24" t="str">
         <f t="shared" si="31"/>
         <v>,</v>
       </c>
-      <c r="Q18" s="25" t="str">
+      <c r="Q18" s="24" t="str">
         <f t="shared" si="31"/>
         <v>6</v>
       </c>
-      <c r="R18" s="25" t="str">
+      <c r="R18" s="24" t="str">
         <f t="shared" si="31"/>
         <v>]</v>
       </c>
@@ -8068,11 +8061,11 @@
         <f t="shared" si="32"/>
         <v>,</v>
       </c>
-      <c r="J19" s="25" t="str">
+      <c r="J19" s="24" t="str">
         <f t="shared" si="32"/>
         <v>1</v>
       </c>
-      <c r="K19" s="25" t="str">
+      <c r="K19" s="24" t="str">
         <f t="shared" si="32"/>
         <v>2</v>
       </c>
@@ -8273,23 +8266,23 @@
         <f t="shared" si="33"/>
         <v>,</v>
       </c>
-      <c r="J20" s="25" t="str">
+      <c r="J20" s="24" t="str">
         <f t="shared" si="33"/>
         <v>[</v>
       </c>
-      <c r="K20" s="25" t="str">
+      <c r="K20" s="24" t="str">
         <f t="shared" si="33"/>
         <v>6</v>
       </c>
-      <c r="L20" s="25" t="str">
+      <c r="L20" s="24" t="str">
         <f t="shared" si="33"/>
         <v>,</v>
       </c>
-      <c r="M20" s="25" t="str">
+      <c r="M20" s="24" t="str">
         <f t="shared" si="33"/>
         <v>6</v>
       </c>
-      <c r="N20" s="25" t="str">
+      <c r="N20" s="24" t="str">
         <f t="shared" si="33"/>
         <v>]</v>
       </c>
@@ -8470,11 +8463,11 @@
         <f t="shared" si="34"/>
         <v>[</v>
       </c>
-      <c r="H21" s="25" t="str">
+      <c r="H21" s="24" t="str">
         <f t="shared" si="34"/>
         <v>1</v>
       </c>
-      <c r="I21" s="25" t="str">
+      <c r="I21" s="24" t="str">
         <f t="shared" si="34"/>
         <v>5</v>
       </c>
@@ -8660,23 +8653,23 @@
         <f t="shared" si="35"/>
         <v>[</v>
       </c>
-      <c r="H22" s="25" t="str">
+      <c r="H22" s="24" t="str">
         <f t="shared" si="35"/>
         <v>[</v>
       </c>
-      <c r="I22" s="25" t="str">
+      <c r="I22" s="24" t="str">
         <f t="shared" si="35"/>
         <v>7</v>
       </c>
-      <c r="J22" s="25" t="str">
+      <c r="J22" s="24" t="str">
         <f t="shared" si="35"/>
         <v>,</v>
       </c>
-      <c r="K22" s="25" t="str">
+      <c r="K22" s="24" t="str">
         <f t="shared" si="35"/>
         <v>8</v>
       </c>
-      <c r="L22" s="25" t="str">
+      <c r="L22" s="24" t="str">
         <f t="shared" si="35"/>
         <v>]</v>
       </c>
@@ -8869,11 +8862,11 @@
         <f t="shared" si="36"/>
         <v>8</v>
       </c>
-      <c r="K23" s="25" t="str">
+      <c r="K23" s="24" t="str">
         <f t="shared" si="36"/>
         <v>]</v>
       </c>
-      <c r="L23" s="25" t="str">
+      <c r="L23" s="24" t="str">
         <f t="shared" si="36"/>
         <v>,</v>
       </c>
@@ -8913,11 +8906,11 @@
         <f t="shared" si="36"/>
         <v>[</v>
       </c>
-      <c r="V23" s="25" t="str">
+      <c r="V23" s="24" t="str">
         <f t="shared" si="36"/>
         <v>2</v>
       </c>
-      <c r="W23" s="25" t="str">
+      <c r="W23" s="24" t="str">
         <f t="shared" si="36"/>
         <v>6</v>
       </c>
@@ -9098,31 +9091,31 @@
         <f t="shared" si="38"/>
         <v>[</v>
       </c>
-      <c r="V24" s="25" t="str">
+      <c r="V24" s="24" t="str">
         <f t="shared" si="38"/>
         <v>[</v>
       </c>
-      <c r="W24" s="25" t="str">
+      <c r="W24" s="24" t="str">
         <f t="shared" si="38"/>
         <v>1</v>
       </c>
-      <c r="X24" s="25" t="str">
+      <c r="X24" s="24" t="str">
         <f t="shared" si="38"/>
         <v>3</v>
       </c>
-      <c r="Y24" s="25" t="str">
+      <c r="Y24" s="24" t="str">
         <f t="shared" si="38"/>
         <v>,</v>
       </c>
-      <c r="Z24" s="25" t="str">
+      <c r="Z24" s="24" t="str">
         <f t="shared" si="38"/>
         <v>1</v>
       </c>
-      <c r="AA24" s="25" t="str">
+      <c r="AA24" s="24" t="str">
         <f t="shared" si="38"/>
         <v>3</v>
       </c>
-      <c r="AB24" s="25" t="str">
+      <c r="AB24" s="24" t="str">
         <f t="shared" si="38"/>
         <v>]</v>
       </c>
@@ -9263,11 +9256,11 @@
         <f t="shared" si="39"/>
         <v>,</v>
       </c>
-      <c r="P25" s="25" t="str">
+      <c r="P25" s="24" t="str">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="Q25" s="25" t="str">
+      <c r="Q25" s="24" t="str">
         <f t="shared" si="39"/>
         <v>9</v>
       </c>
@@ -9452,27 +9445,27 @@
         <f t="shared" si="40"/>
         <v>,</v>
       </c>
-      <c r="P26" s="25" t="str">
+      <c r="P26" s="24" t="str">
         <f t="shared" si="40"/>
         <v>[</v>
       </c>
-      <c r="Q26" s="25" t="str">
+      <c r="Q26" s="24" t="str">
         <f t="shared" si="40"/>
         <v>9</v>
       </c>
-      <c r="R26" s="25" t="str">
+      <c r="R26" s="24" t="str">
         <f t="shared" si="40"/>
         <v>,</v>
       </c>
-      <c r="S26" s="25" t="str">
+      <c r="S26" s="24" t="str">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="T26" s="25" t="str">
+      <c r="T26" s="24" t="str">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="U26" s="25" t="str">
+      <c r="U26" s="24" t="str">
         <f t="shared" si="40"/>
         <v>]</v>
       </c>
@@ -9633,11 +9626,11 @@
         <f t="shared" si="41"/>
         <v>[</v>
       </c>
-      <c r="N27" s="25" t="str">
+      <c r="N27" s="24" t="str">
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
-      <c r="O27" s="25" t="str">
+      <c r="O27" s="24" t="str">
         <f t="shared" si="41"/>
         <v>5</v>
       </c>
@@ -9822,23 +9815,23 @@
         <f t="shared" si="42"/>
         <v>[</v>
       </c>
-      <c r="N28" s="27" t="str">
+      <c r="N28" s="26" t="str">
         <f t="shared" si="42"/>
         <v>[</v>
       </c>
-      <c r="O28" s="27" t="str">
+      <c r="O28" s="26" t="str">
         <f t="shared" si="42"/>
         <v>7</v>
       </c>
-      <c r="P28" s="27" t="str">
+      <c r="P28" s="26" t="str">
         <f t="shared" si="42"/>
         <v>,</v>
       </c>
-      <c r="Q28" s="27" t="str">
+      <c r="Q28" s="26" t="str">
         <f t="shared" si="42"/>
         <v>8</v>
       </c>
-      <c r="R28" s="27" t="str">
+      <c r="R28" s="26" t="str">
         <f t="shared" si="42"/>
         <v>]</v>
       </c>
@@ -9999,11 +9992,11 @@
         <f t="shared" si="43"/>
         <v>,</v>
       </c>
-      <c r="J29" s="27" t="str">
+      <c r="J29" s="26" t="str">
         <f t="shared" si="43"/>
         <v>1</v>
       </c>
-      <c r="K29" s="27" t="str">
+      <c r="K29" s="26" t="str">
         <f t="shared" si="43"/>
         <v>5</v>
       </c>
@@ -10192,23 +10185,23 @@
         <f t="shared" si="44"/>
         <v>,</v>
       </c>
-      <c r="J30" s="27" t="str">
+      <c r="J30" s="26" t="str">
         <f t="shared" si="44"/>
         <v>[</v>
       </c>
-      <c r="K30" s="27" t="str">
+      <c r="K30" s="26" t="str">
         <f t="shared" si="44"/>
         <v>7</v>
       </c>
-      <c r="L30" s="27" t="str">
+      <c r="L30" s="26" t="str">
         <f t="shared" si="44"/>
         <v>,</v>
       </c>
-      <c r="M30" s="27" t="str">
+      <c r="M30" s="26" t="str">
         <f t="shared" si="44"/>
         <v>8</v>
       </c>
-      <c r="N30" s="27" t="str">
+      <c r="N30" s="26" t="str">
         <f t="shared" si="44"/>
         <v>]</v>
       </c>
@@ -10433,11 +10426,11 @@
         <f t="shared" si="45"/>
         <v>[</v>
       </c>
-      <c r="V31" s="27" t="str">
+      <c r="V31" s="26" t="str">
         <f t="shared" si="45"/>
         <v>1</v>
       </c>
-      <c r="W31" s="27" t="str">
+      <c r="W31" s="26" t="str">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
@@ -10626,23 +10619,23 @@
         <f t="shared" si="46"/>
         <v>[</v>
       </c>
-      <c r="V32" s="27" t="str">
+      <c r="V32" s="26" t="str">
         <f t="shared" si="46"/>
         <v>[</v>
       </c>
-      <c r="W32" s="27" t="str">
+      <c r="W32" s="26" t="str">
         <f t="shared" si="46"/>
         <v>5</v>
       </c>
-      <c r="X32" s="27" t="str">
+      <c r="X32" s="26" t="str">
         <f t="shared" si="46"/>
         <v>,</v>
       </c>
-      <c r="Y32" s="27" t="str">
+      <c r="Y32" s="26" t="str">
         <f t="shared" si="46"/>
         <v>5</v>
       </c>
-      <c r="Z32" s="27" t="str">
+      <c r="Z32" s="26" t="str">
         <f t="shared" si="46"/>
         <v>]</v>
       </c>
@@ -10795,11 +10788,11 @@
         <f t="shared" si="47"/>
         <v>,</v>
       </c>
-      <c r="P33" s="27" t="str">
+      <c r="P33" s="26" t="str">
         <f t="shared" si="47"/>
         <v>1</v>
       </c>
-      <c r="Q33" s="27" t="str">
+      <c r="Q33" s="26" t="str">
         <f t="shared" si="47"/>
         <v>3</v>
       </c>
@@ -10988,23 +10981,23 @@
         <f t="shared" si="49"/>
         <v>,</v>
       </c>
-      <c r="P34" s="27" t="str">
+      <c r="P34" s="26" t="str">
         <f t="shared" si="49"/>
         <v>[</v>
       </c>
-      <c r="Q34" s="27" t="str">
+      <c r="Q34" s="26" t="str">
         <f t="shared" si="49"/>
         <v>6</v>
       </c>
-      <c r="R34" s="27" t="str">
+      <c r="R34" s="26" t="str">
         <f t="shared" si="49"/>
         <v>,</v>
       </c>
-      <c r="S34" s="27" t="str">
+      <c r="S34" s="26" t="str">
         <f t="shared" si="49"/>
         <v>7</v>
       </c>
-      <c r="T34" s="27" t="str">
+      <c r="T34" s="26" t="str">
         <f t="shared" si="49"/>
         <v>]</v>
       </c>
@@ -11173,11 +11166,11 @@
         <f t="shared" si="50"/>
         <v>[</v>
       </c>
-      <c r="N35" s="27" t="str">
+      <c r="N35" s="26" t="str">
         <f t="shared" si="50"/>
         <v>1</v>
       </c>
-      <c r="O35" s="27" t="str">
+      <c r="O35" s="26" t="str">
         <f t="shared" si="50"/>
         <v>4</v>
       </c>
@@ -11366,23 +11359,23 @@
         <f t="shared" si="51"/>
         <v>[</v>
       </c>
-      <c r="N36" s="27" t="str">
+      <c r="N36" s="26" t="str">
         <f t="shared" si="51"/>
         <v>[</v>
       </c>
-      <c r="O36" s="27" t="str">
+      <c r="O36" s="26" t="str">
         <f t="shared" si="51"/>
         <v>7</v>
       </c>
-      <c r="P36" s="27" t="str">
+      <c r="P36" s="26" t="str">
         <f t="shared" si="51"/>
         <v>,</v>
       </c>
-      <c r="Q36" s="27" t="str">
+      <c r="Q36" s="26" t="str">
         <f t="shared" si="51"/>
         <v>7</v>
       </c>
-      <c r="R36" s="27" t="str">
+      <c r="R36" s="26" t="str">
         <f t="shared" si="51"/>
         <v>]</v>
       </c>
@@ -11599,11 +11592,11 @@
         <f t="shared" si="52"/>
         <v>,</v>
       </c>
-      <c r="X37" s="27" t="str">
+      <c r="X37" s="26" t="str">
         <f t="shared" si="52"/>
         <v>1</v>
       </c>
-      <c r="Y37" s="27" t="str">
+      <c r="Y37" s="26" t="str">
         <f t="shared" si="52"/>
         <v>8</v>
       </c>
@@ -11792,23 +11785,23 @@
         <f t="shared" si="53"/>
         <v>,</v>
       </c>
-      <c r="X38" s="27" t="str">
+      <c r="X38" s="26" t="str">
         <f t="shared" si="53"/>
         <v>[</v>
       </c>
-      <c r="Y38" s="27" t="str">
+      <c r="Y38" s="26" t="str">
         <f t="shared" si="53"/>
         <v>9</v>
       </c>
-      <c r="Z38" s="27" t="str">
+      <c r="Z38" s="26" t="str">
         <f t="shared" si="53"/>
         <v>,</v>
       </c>
-      <c r="AA38" s="27" t="str">
+      <c r="AA38" s="26" t="str">
         <f t="shared" si="53"/>
         <v>9</v>
       </c>
-      <c r="AB38" s="27" t="str">
+      <c r="AB38" s="26" t="str">
         <f t="shared" si="53"/>
         <v>]</v>
       </c>
@@ -11977,11 +11970,11 @@
         <f t="shared" si="54"/>
         <v>[</v>
       </c>
-      <c r="V39" s="27" t="str">
+      <c r="V39" s="26" t="str">
         <f t="shared" si="54"/>
         <v>1</v>
       </c>
-      <c r="W39" s="27" t="str">
+      <c r="W39" s="26" t="str">
         <f t="shared" si="54"/>
         <v>6</v>
       </c>
@@ -12170,23 +12163,23 @@
         <f t="shared" si="55"/>
         <v>[</v>
       </c>
-      <c r="V40" s="27" t="str">
+      <c r="V40" s="26" t="str">
         <f t="shared" si="55"/>
         <v>[</v>
       </c>
-      <c r="W40" s="27" t="str">
+      <c r="W40" s="26" t="str">
         <f t="shared" si="55"/>
         <v>8</v>
       </c>
-      <c r="X40" s="27" t="str">
+      <c r="X40" s="26" t="str">
         <f t="shared" si="55"/>
         <v>,</v>
       </c>
-      <c r="Y40" s="27" t="str">
+      <c r="Y40" s="26" t="str">
         <f t="shared" si="55"/>
         <v>8</v>
       </c>
-      <c r="Z40" s="27" t="str">
+      <c r="Z40" s="26" t="str">
         <f t="shared" si="55"/>
         <v>]</v>
       </c>
@@ -12339,11 +12332,11 @@
         <f t="shared" si="57"/>
         <v>,</v>
       </c>
-      <c r="P41" s="27" t="str">
+      <c r="P41" s="26" t="str">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="Q41" s="27" t="str">
+      <c r="Q41" s="26" t="str">
         <f t="shared" si="57"/>
         <v>5</v>
       </c>
@@ -12536,23 +12529,23 @@
         <f t="shared" si="59"/>
         <v>,</v>
       </c>
-      <c r="P42" s="27" t="str">
+      <c r="P42" s="26" t="str">
         <f t="shared" si="59"/>
         <v>[</v>
       </c>
-      <c r="Q42" s="27" t="str">
+      <c r="Q42" s="26" t="str">
         <f t="shared" si="59"/>
         <v>7</v>
       </c>
-      <c r="R42" s="27" t="str">
+      <c r="R42" s="26" t="str">
         <f t="shared" si="59"/>
         <v>,</v>
       </c>
-      <c r="S42" s="27" t="str">
+      <c r="S42" s="26" t="str">
         <f t="shared" si="59"/>
         <v>8</v>
       </c>
-      <c r="T42" s="27" t="str">
+      <c r="T42" s="26" t="str">
         <f t="shared" si="59"/>
         <v>]</v>
       </c>
@@ -12773,11 +12766,11 @@
         <f t="shared" si="60"/>
         <v>[</v>
       </c>
-      <c r="AB43" s="27" t="str">
+      <c r="AB43" s="26" t="str">
         <f t="shared" si="60"/>
         <v>3</v>
       </c>
-      <c r="AC43" s="27" t="str">
+      <c r="AC43" s="26" t="str">
         <f t="shared" si="60"/>
         <v>4</v>
       </c>
@@ -12970,31 +12963,31 @@
         <f t="shared" si="61"/>
         <v>[</v>
       </c>
-      <c r="AB44" s="27" t="str">
+      <c r="AB44" s="26" t="str">
         <f t="shared" si="61"/>
         <v>[</v>
       </c>
-      <c r="AC44" s="27" t="str">
+      <c r="AC44" s="26" t="str">
         <f t="shared" si="61"/>
         <v>1</v>
       </c>
-      <c r="AD44" s="27" t="str">
+      <c r="AD44" s="26" t="str">
         <f t="shared" si="61"/>
         <v>7</v>
       </c>
-      <c r="AE44" s="27" t="str">
+      <c r="AE44" s="26" t="str">
         <f t="shared" si="61"/>
         <v>,</v>
       </c>
-      <c r="AF44" s="27" t="str">
+      <c r="AF44" s="26" t="str">
         <f t="shared" si="61"/>
         <v>1</v>
       </c>
-      <c r="AG44" s="27" t="str">
+      <c r="AG44" s="26" t="str">
         <f t="shared" si="61"/>
         <v>7</v>
       </c>
-      <c r="AH44" s="27" t="str">
+      <c r="AH44" s="26" t="str">
         <f t="shared" si="61"/>
         <v>]</v>
       </c>
@@ -13151,11 +13144,11 @@
         <f t="shared" si="62"/>
         <v>,</v>
       </c>
-      <c r="X45" s="27" t="str">
+      <c r="X45" s="26" t="str">
         <f t="shared" si="62"/>
         <v>2</v>
       </c>
-      <c r="Y45" s="27" t="str">
+      <c r="Y45" s="26" t="str">
         <f t="shared" si="62"/>
         <v>5</v>
       </c>
@@ -13348,31 +13341,31 @@
         <f t="shared" si="63"/>
         <v>,</v>
       </c>
-      <c r="X46" s="27" t="str">
+      <c r="X46" s="26" t="str">
         <f t="shared" si="63"/>
         <v>[</v>
       </c>
-      <c r="Y46" s="27" t="str">
+      <c r="Y46" s="26" t="str">
         <f t="shared" si="63"/>
         <v>1</v>
       </c>
-      <c r="Z46" s="27" t="str">
+      <c r="Z46" s="26" t="str">
         <f t="shared" si="63"/>
         <v>2</v>
       </c>
-      <c r="AA46" s="27" t="str">
+      <c r="AA46" s="26" t="str">
         <f t="shared" si="63"/>
         <v>,</v>
       </c>
-      <c r="AB46" s="27" t="str">
+      <c r="AB46" s="26" t="str">
         <f t="shared" si="63"/>
         <v>1</v>
       </c>
-      <c r="AC46" s="27" t="str">
+      <c r="AC46" s="26" t="str">
         <f t="shared" si="63"/>
         <v>3</v>
       </c>
-      <c r="AD46" s="27" t="str">
+      <c r="AD46" s="26" t="str">
         <f t="shared" si="63"/>
         <v>]</v>
       </c>
@@ -13537,11 +13530,11 @@
         <f t="shared" si="65"/>
         <v>[</v>
       </c>
-      <c r="V47" s="27" t="str">
+      <c r="V47" s="26" t="str">
         <f t="shared" si="65"/>
         <v>2</v>
       </c>
-      <c r="W47" s="27" t="str">
+      <c r="W47" s="26" t="str">
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
@@ -13750,31 +13743,31 @@
         <f t="shared" si="67"/>
         <v>[</v>
       </c>
-      <c r="V48" s="27" t="str">
+      <c r="V48" s="26" t="str">
         <f t="shared" si="67"/>
         <v>[</v>
       </c>
-      <c r="W48" s="27" t="str">
+      <c r="W48" s="26" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="X48" s="27" t="str">
+      <c r="X48" s="26" t="str">
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
-      <c r="Y48" s="27" t="str">
+      <c r="Y48" s="26" t="str">
         <f t="shared" si="67"/>
         <v>,</v>
       </c>
-      <c r="Z48" s="27" t="str">
+      <c r="Z48" s="26" t="str">
         <f t="shared" si="67"/>
         <v>1</v>
       </c>
-      <c r="AA48" s="27" t="str">
+      <c r="AA48" s="26" t="str">
         <f t="shared" si="67"/>
         <v>0</v>
       </c>
-      <c r="AB48" s="27" t="str">
+      <c r="AB48" s="26" t="str">
         <f t="shared" si="67"/>
         <v>]</v>
       </c>
@@ -13939,11 +13932,11 @@
         <f t="shared" si="69"/>
         <v>,</v>
       </c>
-      <c r="P49" s="27" t="str">
+      <c r="P49" s="26" t="str">
         <f t="shared" si="69"/>
         <v>1</v>
       </c>
-      <c r="Q49" s="27" t="str">
+      <c r="Q49" s="26" t="str">
         <f t="shared" si="69"/>
         <v>0</v>
       </c>
@@ -14152,27 +14145,27 @@
         <f t="shared" si="71"/>
         <v>,</v>
       </c>
-      <c r="P50" s="27" t="str">
+      <c r="P50" s="26" t="str">
         <f t="shared" si="71"/>
         <v>[</v>
       </c>
-      <c r="Q50" s="27" t="str">
+      <c r="Q50" s="26" t="str">
         <f t="shared" si="71"/>
         <v>5</v>
       </c>
-      <c r="R50" s="27" t="str">
+      <c r="R50" s="26" t="str">
         <f t="shared" si="71"/>
         <v>,</v>
       </c>
-      <c r="S50" s="27" t="str">
+      <c r="S50" s="26" t="str">
         <f t="shared" si="71"/>
         <v>5</v>
       </c>
-      <c r="T50" s="27" t="str">
+      <c r="T50" s="26" t="str">
         <f t="shared" si="71"/>
         <v>]</v>
       </c>
-      <c r="U50" s="27" t="str">
+      <c r="U50" s="26" t="str">
         <f t="shared" si="71"/>
         <v>]</v>
       </c>
@@ -14357,11 +14350,11 @@
         <f t="shared" si="73"/>
         <v>[</v>
       </c>
-      <c r="N51" s="27" t="str">
+      <c r="N51" s="26" t="str">
         <f t="shared" si="73"/>
         <v>1</v>
       </c>
-      <c r="O51" s="27" t="str">
+      <c r="O51" s="26" t="str">
         <f t="shared" si="73"/>
         <v>2</v>
       </c>
@@ -14570,23 +14563,23 @@
         <f t="shared" si="76"/>
         <v>[</v>
       </c>
-      <c r="N52" s="27" t="str">
+      <c r="N52" s="26" t="str">
         <f t="shared" si="76"/>
         <v>[</v>
       </c>
-      <c r="O52" s="27" t="str">
+      <c r="O52" s="26" t="str">
         <f t="shared" si="76"/>
         <v>6</v>
       </c>
-      <c r="P52" s="27" t="str">
+      <c r="P52" s="26" t="str">
         <f t="shared" si="76"/>
         <v>,</v>
       </c>
-      <c r="Q52" s="27" t="str">
+      <c r="Q52" s="26" t="str">
         <f t="shared" si="76"/>
         <v>6</v>
       </c>
-      <c r="R52" s="27" t="str">
+      <c r="R52" s="26" t="str">
         <f t="shared" si="76"/>
         <v>]</v>
       </c>
@@ -14767,11 +14760,11 @@
         <f t="shared" si="79"/>
         <v>,</v>
       </c>
-      <c r="J53" s="27" t="str">
+      <c r="J53" s="26" t="str">
         <f t="shared" si="79"/>
         <v>1</v>
       </c>
-      <c r="K53" s="27" t="str">
+      <c r="K53" s="26" t="str">
         <f t="shared" si="79"/>
         <v>3</v>
       </c>
@@ -14980,23 +14973,23 @@
         <f t="shared" si="82"/>
         <v>,</v>
       </c>
-      <c r="J54" s="27" t="str">
+      <c r="J54" s="26" t="str">
         <f t="shared" si="82"/>
         <v>[</v>
       </c>
-      <c r="K54" s="27" t="str">
+      <c r="K54" s="26" t="str">
         <f t="shared" si="82"/>
         <v>6</v>
       </c>
-      <c r="L54" s="27" t="str">
+      <c r="L54" s="26" t="str">
         <f t="shared" si="82"/>
         <v>,</v>
       </c>
-      <c r="M54" s="27" t="str">
+      <c r="M54" s="26" t="str">
         <f t="shared" si="82"/>
         <v>7</v>
       </c>
-      <c r="N54" s="27" t="str">
+      <c r="N54" s="26" t="str">
         <f t="shared" si="82"/>
         <v>]</v>
       </c>
@@ -15185,11 +15178,11 @@
         <f t="shared" si="85"/>
         <v>[</v>
       </c>
-      <c r="H55" s="27" t="str">
+      <c r="H55" s="26" t="str">
         <f t="shared" si="85"/>
         <v>1</v>
       </c>
-      <c r="I55" s="27" t="str">
+      <c r="I55" s="26" t="str">
         <f t="shared" si="85"/>
         <v>3</v>
       </c>
@@ -15380,7 +15373,7 @@
         <v>0</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
       <c r="D56" s="18" t="str">
         <f>MID($C$56,D1,1)</f>
@@ -15398,23 +15391,23 @@
         <f t="shared" si="88"/>
         <v>[</v>
       </c>
-      <c r="H56" s="27" t="str">
+      <c r="H56" s="26" t="str">
         <f t="shared" si="88"/>
         <v>[</v>
       </c>
-      <c r="I56" s="27" t="str">
+      <c r="I56" s="26" t="str">
         <f t="shared" si="88"/>
         <v>6</v>
       </c>
-      <c r="J56" s="27" t="str">
+      <c r="J56" s="26" t="str">
         <f t="shared" si="88"/>
         <v>,</v>
       </c>
-      <c r="K56" s="27" t="str">
+      <c r="K56" s="26" t="str">
         <f t="shared" si="88"/>
-        <v>6</v>
-      </c>
-      <c r="L56" s="27" t="str">
+        <v>7</v>
+      </c>
+      <c r="L56" s="26" t="str">
         <f t="shared" si="88"/>
         <v>]</v>
       </c>
@@ -15593,7 +15586,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="D57" s="18" t="str">
         <f>MID($C$57,D1,1)</f>
@@ -15619,11 +15612,11 @@
         <f t="shared" si="91"/>
         <v>,</v>
       </c>
-      <c r="J57" s="18" t="str">
+      <c r="J57" s="29" t="str">
         <f t="shared" si="91"/>
-        <v>6</v>
-      </c>
-      <c r="K57" s="18" t="str">
+        <v>7</v>
+      </c>
+      <c r="K57" s="29" t="str">
         <f t="shared" si="91"/>
         <v>]</v>
       </c>
@@ -15675,11 +15668,11 @@
         <f t="shared" si="91"/>
         <v>,</v>
       </c>
-      <c r="X57" s="27" t="str">
+      <c r="X57" s="26" t="str">
         <f t="shared" si="91"/>
         <v>1</v>
       </c>
-      <c r="Y57" s="27" t="str">
+      <c r="Y57" s="26" t="str">
         <f t="shared" si="91"/>
         <v>0</v>
       </c>
@@ -15806,7 +15799,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D58" s="18" t="str">
         <f>MID($C$58,D1,1)</f>
@@ -15888,23 +15881,23 @@
         <f t="shared" si="93"/>
         <v>,</v>
       </c>
-      <c r="X58" s="27" t="str">
+      <c r="X58" s="26" t="str">
         <f t="shared" si="93"/>
         <v>[</v>
       </c>
-      <c r="Y58" s="27" t="str">
+      <c r="Y58" s="26" t="str">
         <f t="shared" si="93"/>
         <v>5</v>
       </c>
-      <c r="Z58" s="27" t="str">
+      <c r="Z58" s="26" t="str">
         <f t="shared" si="93"/>
         <v>,</v>
       </c>
-      <c r="AA58" s="27" t="str">
+      <c r="AA58" s="26" t="str">
         <f t="shared" si="93"/>
         <v>5</v>
       </c>
-      <c r="AB58" s="27" t="str">
+      <c r="AB58" s="26" t="str">
         <f t="shared" si="93"/>
         <v>]</v>
       </c>
@@ -16019,7 +16012,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D59" s="18" t="str">
         <f>MID($C$59,D1,1)</f>
@@ -16093,11 +16086,11 @@
         <f t="shared" si="96"/>
         <v>[</v>
       </c>
-      <c r="V59" s="27" t="str">
+      <c r="V59" s="26" t="str">
         <f t="shared" si="96"/>
         <v>1</v>
       </c>
-      <c r="W59" s="27" t="str">
+      <c r="W59" s="26" t="str">
         <f t="shared" si="96"/>
         <v>0</v>
       </c>
@@ -16232,7 +16225,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D60" s="18" t="str">
         <f>MID($C$60,D1,1)</f>
@@ -16306,23 +16299,23 @@
         <f t="shared" si="99"/>
         <v>[</v>
       </c>
-      <c r="V60" s="27" t="str">
+      <c r="V60" s="26" t="str">
         <f t="shared" si="99"/>
         <v>[</v>
       </c>
-      <c r="W60" s="27" t="str">
+      <c r="W60" s="26" t="str">
         <f t="shared" si="99"/>
         <v>5</v>
       </c>
-      <c r="X60" s="27" t="str">
+      <c r="X60" s="26" t="str">
         <f t="shared" si="99"/>
         <v>,</v>
       </c>
-      <c r="Y60" s="27" t="str">
+      <c r="Y60" s="26" t="str">
         <f t="shared" si="99"/>
         <v>5</v>
       </c>
-      <c r="Z60" s="27" t="str">
+      <c r="Z60" s="26" t="str">
         <f t="shared" si="99"/>
         <v>]</v>
       </c>
@@ -16445,7 +16438,7 @@
         <v>0</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D61" s="18" t="str">
         <f>MID($C$61,D1,1)</f>
@@ -16495,11 +16488,11 @@
         <f t="shared" si="102"/>
         <v>,</v>
       </c>
-      <c r="P61" s="27" t="str">
+      <c r="P61" s="26" t="str">
         <f t="shared" si="102"/>
         <v>1</v>
       </c>
-      <c r="Q61" s="27" t="str">
+      <c r="Q61" s="26" t="str">
         <f t="shared" si="102"/>
         <v>1</v>
       </c>
@@ -16658,7 +16651,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D62" s="18" t="str">
         <f>MID($C$62,D1,1)</f>
@@ -16708,23 +16701,23 @@
         <f t="shared" si="105"/>
         <v>,</v>
       </c>
-      <c r="P62" s="27" t="str">
+      <c r="P62" s="26" t="str">
         <f t="shared" si="105"/>
         <v>[</v>
       </c>
-      <c r="Q62" s="27" t="str">
+      <c r="Q62" s="26" t="str">
         <f t="shared" si="105"/>
         <v>5</v>
       </c>
-      <c r="R62" s="27" t="str">
+      <c r="R62" s="26" t="str">
         <f t="shared" si="105"/>
         <v>,</v>
       </c>
-      <c r="S62" s="27" t="str">
+      <c r="S62" s="26" t="str">
         <f t="shared" si="105"/>
         <v>6</v>
       </c>
-      <c r="T62" s="27" t="str">
+      <c r="T62" s="26" t="str">
         <f t="shared" si="105"/>
         <v>]</v>
       </c>
@@ -16871,7 +16864,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="20" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D63" s="18" t="str">
         <f>MID($C$63,D1,1)</f>
@@ -16913,11 +16906,11 @@
         <f t="shared" si="108"/>
         <v>[</v>
       </c>
-      <c r="N63" s="27" t="str">
+      <c r="N63" s="26" t="str">
         <f t="shared" si="108"/>
         <v>1</v>
       </c>
-      <c r="O63" s="27" t="str">
+      <c r="O63" s="26" t="str">
         <f t="shared" si="108"/>
         <v>2</v>
       </c>
@@ -17084,7 +17077,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D64" s="18" t="str">
         <f>MID($C$64,D1,1)</f>
@@ -17126,23 +17119,23 @@
         <f t="shared" si="111"/>
         <v>[</v>
       </c>
-      <c r="N64" s="27" t="str">
+      <c r="N64" s="26" t="str">
         <f t="shared" si="111"/>
         <v>[</v>
       </c>
-      <c r="O64" s="27" t="str">
+      <c r="O64" s="26" t="str">
         <f t="shared" si="111"/>
         <v>6</v>
       </c>
-      <c r="P64" s="27" t="str">
+      <c r="P64" s="26" t="str">
         <f t="shared" si="111"/>
         <v>,</v>
       </c>
-      <c r="Q64" s="27" t="str">
+      <c r="Q64" s="26" t="str">
         <f t="shared" si="111"/>
         <v>6</v>
       </c>
-      <c r="R64" s="27" t="str">
+      <c r="R64" s="26" t="str">
         <f t="shared" si="111"/>
         <v>]</v>
       </c>
@@ -17297,7 +17290,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D65" s="18" t="str">
         <f>MID($C$65,D1,1)</f>
@@ -17323,11 +17316,11 @@
         <f t="shared" si="114"/>
         <v>,</v>
       </c>
-      <c r="J65" s="27" t="str">
+      <c r="J65" s="26" t="str">
         <f t="shared" si="114"/>
         <v>1</v>
       </c>
-      <c r="K65" s="27" t="str">
+      <c r="K65" s="26" t="str">
         <f t="shared" si="114"/>
         <v>2</v>
       </c>
@@ -17510,7 +17503,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D66" s="18" t="str">
         <f>MID($C$66,D1,1)</f>
@@ -17536,23 +17529,23 @@
         <f t="shared" si="117"/>
         <v>,</v>
       </c>
-      <c r="J66" s="27" t="str">
+      <c r="J66" s="26" t="str">
         <f t="shared" si="117"/>
         <v>[</v>
       </c>
-      <c r="K66" s="27" t="str">
+      <c r="K66" s="26" t="str">
         <f t="shared" si="117"/>
         <v>6</v>
       </c>
-      <c r="L66" s="27" t="str">
+      <c r="L66" s="26" t="str">
         <f t="shared" si="117"/>
         <v>,</v>
       </c>
-      <c r="M66" s="27" t="str">
+      <c r="M66" s="26" t="str">
         <f t="shared" si="117"/>
         <v>6</v>
       </c>
-      <c r="N66" s="27" t="str">
+      <c r="N66" s="26" t="str">
         <f t="shared" si="117"/>
         <v>]</v>
       </c>
@@ -17707,7 +17700,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D67" s="18" t="str">
         <f>MID($C$67,D1,1)</f>
@@ -17805,11 +17798,11 @@
         <f t="shared" si="118"/>
         <v>[</v>
       </c>
-      <c r="AB67" s="27" t="str">
+      <c r="AB67" s="26" t="str">
         <f t="shared" si="118"/>
         <v>1</v>
       </c>
-      <c r="AC67" s="27" t="str">
+      <c r="AC67" s="26" t="str">
         <f t="shared" si="118"/>
         <v>8</v>
       </c>
@@ -17900,7 +17893,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D68" s="18" t="str">
         <f>MID($C$68,D1,1)</f>
@@ -17998,23 +17991,23 @@
         <f t="shared" si="119"/>
         <v>[</v>
       </c>
-      <c r="AB68" s="27" t="str">
+      <c r="AB68" s="26" t="str">
         <f t="shared" si="119"/>
         <v>[</v>
       </c>
-      <c r="AC68" s="27" t="str">
+      <c r="AC68" s="26" t="str">
         <f t="shared" si="119"/>
         <v>9</v>
       </c>
-      <c r="AD68" s="27" t="str">
+      <c r="AD68" s="26" t="str">
         <f t="shared" si="119"/>
         <v>,</v>
       </c>
-      <c r="AE68" s="27" t="str">
+      <c r="AE68" s="26" t="str">
         <f t="shared" si="119"/>
         <v>9</v>
       </c>
-      <c r="AF68" s="27" t="str">
+      <c r="AF68" s="26" t="str">
         <f t="shared" si="119"/>
         <v>]</v>
       </c>
@@ -18093,7 +18086,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D69" s="18" t="str">
         <f>MID($C$69,D1,1)</f>
@@ -18175,11 +18168,11 @@
         <f t="shared" si="120"/>
         <v>,</v>
       </c>
-      <c r="X69" s="27" t="str">
+      <c r="X69" s="26" t="str">
         <f t="shared" si="120"/>
         <v>1</v>
       </c>
-      <c r="Y69" s="27" t="str">
+      <c r="Y69" s="26" t="str">
         <f t="shared" si="120"/>
         <v>4</v>
       </c>
@@ -18286,7 +18279,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D70" s="18" t="str">
         <f>MID($C$70,D1,1)</f>
@@ -18368,23 +18361,23 @@
         <f t="shared" si="121"/>
         <v>,</v>
       </c>
-      <c r="X70" s="27" t="str">
+      <c r="X70" s="26" t="str">
         <f t="shared" si="121"/>
         <v>[</v>
       </c>
-      <c r="Y70" s="27" t="str">
+      <c r="Y70" s="26" t="str">
         <f t="shared" si="121"/>
         <v>7</v>
       </c>
-      <c r="Z70" s="27" t="str">
+      <c r="Z70" s="26" t="str">
         <f t="shared" si="121"/>
         <v>,</v>
       </c>
-      <c r="AA70" s="27" t="str">
+      <c r="AA70" s="26" t="str">
         <f t="shared" si="121"/>
         <v>7</v>
       </c>
-      <c r="AB70" s="27" t="str">
+      <c r="AB70" s="26" t="str">
         <f t="shared" si="121"/>
         <v>]</v>
       </c>
@@ -18479,7 +18472,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D71" s="18" t="str">
         <f>MID($C$71,D1,1)</f>
@@ -18553,11 +18546,11 @@
         <f t="shared" si="123"/>
         <v>[</v>
       </c>
-      <c r="V71" s="27" t="str">
+      <c r="V71" s="26" t="str">
         <f t="shared" si="123"/>
         <v>1</v>
       </c>
-      <c r="W71" s="27" t="str">
+      <c r="W71" s="26" t="str">
         <f t="shared" si="123"/>
         <v>3</v>
       </c>
@@ -18672,7 +18665,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D72" s="18" t="str">
         <f>MID($C$72,D1,1)</f>
@@ -18746,23 +18739,23 @@
         <f t="shared" si="124"/>
         <v>[</v>
       </c>
-      <c r="V72" s="27" t="str">
+      <c r="V72" s="26" t="str">
         <f t="shared" si="124"/>
         <v>[</v>
       </c>
-      <c r="W72" s="27" t="str">
+      <c r="W72" s="26" t="str">
         <f t="shared" si="124"/>
         <v>6</v>
       </c>
-      <c r="X72" s="27" t="str">
+      <c r="X72" s="26" t="str">
         <f t="shared" si="124"/>
         <v>,</v>
       </c>
-      <c r="Y72" s="27" t="str">
+      <c r="Y72" s="26" t="str">
         <f t="shared" si="124"/>
         <v>7</v>
       </c>
-      <c r="Z72" s="27" t="str">
+      <c r="Z72" s="26" t="str">
         <f t="shared" si="124"/>
         <v>]</v>
       </c>
@@ -18865,7 +18858,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D73" s="18" t="str">
         <f>MID($C$73,D1,1)</f>
@@ -18915,11 +18908,11 @@
         <f t="shared" si="125"/>
         <v>,</v>
       </c>
-      <c r="P73" s="27" t="str">
+      <c r="P73" s="26" t="str">
         <f t="shared" si="125"/>
         <v>1</v>
       </c>
-      <c r="Q73" s="27" t="str">
+      <c r="Q73" s="26" t="str">
         <f t="shared" si="125"/>
         <v>2</v>
       </c>
@@ -19058,7 +19051,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D74" s="18" t="str">
         <f>MID($C$74,D1,1)</f>
@@ -19108,23 +19101,23 @@
         <f t="shared" si="126"/>
         <v>,</v>
       </c>
-      <c r="P74" s="27" t="str">
+      <c r="P74" s="26" t="str">
         <f t="shared" si="126"/>
         <v>[</v>
       </c>
-      <c r="Q74" s="27" t="str">
+      <c r="Q74" s="26" t="str">
         <f t="shared" si="126"/>
         <v>6</v>
       </c>
-      <c r="R74" s="27" t="str">
+      <c r="R74" s="26" t="str">
         <f t="shared" si="126"/>
         <v>,</v>
       </c>
-      <c r="S74" s="27" t="str">
+      <c r="S74" s="26" t="str">
         <f t="shared" si="126"/>
         <v>6</v>
       </c>
-      <c r="T74" s="27" t="str">
+      <c r="T74" s="26" t="str">
         <f t="shared" si="126"/>
         <v>]</v>
       </c>
@@ -19251,7 +19244,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D75" s="18" t="str">
         <f>MID($C$75,D1,1)</f>
@@ -19293,11 +19286,11 @@
         <f t="shared" si="127"/>
         <v>[</v>
       </c>
-      <c r="N75" s="27" t="str">
+      <c r="N75" s="26" t="str">
         <f t="shared" si="127"/>
         <v>1</v>
       </c>
-      <c r="O75" s="27" t="str">
+      <c r="O75" s="26" t="str">
         <f t="shared" si="127"/>
         <v>2</v>
       </c>
@@ -19444,7 +19437,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D76" s="18" t="str">
         <f>MID($C$76,D1,1)</f>
@@ -19550,11 +19543,11 @@
         <f t="shared" si="128"/>
         <v>,</v>
       </c>
-      <c r="AD76" s="27" t="str">
+      <c r="AD76" s="26" t="str">
         <f t="shared" si="128"/>
         <v>2</v>
       </c>
-      <c r="AE76" s="27" t="str">
+      <c r="AE76" s="26" t="str">
         <f t="shared" si="128"/>
         <v>6</v>
       </c>
@@ -19637,7 +19630,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D77" s="18" t="str">
         <f>MID($C$77,D1,1)</f>
@@ -19743,31 +19736,31 @@
         <f t="shared" si="130"/>
         <v>,</v>
       </c>
-      <c r="AD77" s="27" t="str">
+      <c r="AD77" s="26" t="str">
         <f t="shared" si="130"/>
         <v>[</v>
       </c>
-      <c r="AE77" s="27" t="str">
+      <c r="AE77" s="26" t="str">
         <f t="shared" si="130"/>
         <v>1</v>
       </c>
-      <c r="AF77" s="27" t="str">
+      <c r="AF77" s="26" t="str">
         <f t="shared" si="130"/>
         <v>3</v>
       </c>
-      <c r="AG77" s="27" t="str">
+      <c r="AG77" s="26" t="str">
         <f t="shared" si="130"/>
         <v>,</v>
       </c>
-      <c r="AH77" s="27" t="str">
+      <c r="AH77" s="26" t="str">
         <f t="shared" si="130"/>
         <v>1</v>
       </c>
-      <c r="AI77" s="27" t="str">
+      <c r="AI77" s="26" t="str">
         <f t="shared" si="130"/>
         <v>3</v>
       </c>
-      <c r="AJ77" s="27" t="str">
+      <c r="AJ77" s="26" t="str">
         <f t="shared" si="130"/>
         <v>]</v>
       </c>
@@ -19838,7 +19831,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D78" s="18" t="str">
         <f>MID($C$78,D1,1)</f>
@@ -19936,11 +19929,11 @@
         <f t="shared" si="131"/>
         <v>[</v>
       </c>
-      <c r="AB78" s="27" t="str">
+      <c r="AB78" s="26" t="str">
         <f t="shared" si="131"/>
         <v>2</v>
       </c>
-      <c r="AC78" s="27" t="str">
+      <c r="AC78" s="26" t="str">
         <f t="shared" si="131"/>
         <v>0</v>
       </c>
@@ -20039,7 +20032,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D79" s="18" t="str">
         <f>MID($C$79,D1,1)</f>
@@ -20137,31 +20130,31 @@
         <f t="shared" si="132"/>
         <v>[</v>
       </c>
-      <c r="AB79" s="27" t="str">
+      <c r="AB79" s="26" t="str">
         <f t="shared" si="132"/>
         <v>[</v>
       </c>
-      <c r="AC79" s="27" t="str">
+      <c r="AC79" s="26" t="str">
         <f t="shared" si="132"/>
         <v>1</v>
       </c>
-      <c r="AD79" s="27" t="str">
+      <c r="AD79" s="26" t="str">
         <f t="shared" si="132"/>
         <v>0</v>
       </c>
-      <c r="AE79" s="27" t="str">
+      <c r="AE79" s="26" t="str">
         <f t="shared" si="132"/>
         <v>,</v>
       </c>
-      <c r="AF79" s="27" t="str">
+      <c r="AF79" s="26" t="str">
         <f t="shared" si="132"/>
         <v>1</v>
       </c>
-      <c r="AG79" s="27" t="str">
+      <c r="AG79" s="26" t="str">
         <f t="shared" si="132"/>
         <v>0</v>
       </c>
-      <c r="AH79" s="27" t="str">
+      <c r="AH79" s="26" t="str">
         <f t="shared" si="132"/>
         <v>]</v>
       </c>
@@ -20240,7 +20233,7 @@
         <v>0</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D80" s="18" t="str">
         <f>MID($C$80,D1,1)</f>
@@ -20322,11 +20315,11 @@
         <f t="shared" si="133"/>
         <v>,</v>
       </c>
-      <c r="X80" s="27" t="str">
+      <c r="X80" s="26" t="str">
         <f t="shared" si="133"/>
         <v>1</v>
       </c>
-      <c r="Y80" s="27" t="str">
+      <c r="Y80" s="26" t="str">
         <f t="shared" si="133"/>
         <v>7</v>
       </c>
@@ -20441,7 +20434,7 @@
         <v>0</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D81" s="18" t="str">
         <f>MID($C$81,D1,1)</f>
@@ -20523,23 +20516,23 @@
         <f t="shared" si="134"/>
         <v>,</v>
       </c>
-      <c r="X81" s="27" t="str">
+      <c r="X81" s="26" t="str">
         <f t="shared" si="134"/>
         <v>[</v>
       </c>
-      <c r="Y81" s="27" t="str">
+      <c r="Y81" s="26" t="str">
         <f t="shared" si="134"/>
         <v>8</v>
       </c>
-      <c r="Z81" s="27" t="str">
+      <c r="Z81" s="26" t="str">
         <f t="shared" si="134"/>
         <v>,</v>
       </c>
-      <c r="AA81" s="27" t="str">
+      <c r="AA81" s="26" t="str">
         <f t="shared" si="134"/>
         <v>9</v>
       </c>
-      <c r="AB81" s="27" t="str">
+      <c r="AB81" s="26" t="str">
         <f t="shared" si="134"/>
         <v>]</v>
       </c>
@@ -20642,7 +20635,7 @@
         <v>0</v>
       </c>
       <c r="C82" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D82" s="18" t="str">
         <f>MID($C$82,D1,1)</f>
@@ -20716,11 +20709,11 @@
         <f t="shared" si="135"/>
         <v>[</v>
       </c>
-      <c r="V82" s="27" t="str">
+      <c r="V82" s="26" t="str">
         <f t="shared" si="135"/>
         <v>1</v>
       </c>
-      <c r="W82" s="27" t="str">
+      <c r="W82" s="26" t="str">
         <f t="shared" si="135"/>
         <v>4</v>
       </c>
@@ -20843,7 +20836,7 @@
         <v>0</v>
       </c>
       <c r="C83" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D83" s="18" t="str">
         <f>MID($C$83,D1,1)</f>
@@ -20917,23 +20910,23 @@
         <f t="shared" si="136"/>
         <v>[</v>
       </c>
-      <c r="V83" s="27" t="str">
+      <c r="V83" s="26" t="str">
         <f t="shared" si="136"/>
         <v>[</v>
       </c>
-      <c r="W83" s="27" t="str">
+      <c r="W83" s="26" t="str">
         <f t="shared" si="136"/>
         <v>7</v>
       </c>
-      <c r="X83" s="27" t="str">
+      <c r="X83" s="26" t="str">
         <f t="shared" si="136"/>
         <v>,</v>
       </c>
-      <c r="Y83" s="27" t="str">
+      <c r="Y83" s="26" t="str">
         <f t="shared" si="136"/>
         <v>7</v>
       </c>
-      <c r="Z83" s="27" t="str">
+      <c r="Z83" s="26" t="str">
         <f t="shared" si="136"/>
         <v>]</v>
       </c>
@@ -21044,7 +21037,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D84" s="18" t="str">
         <f>MID($C$84,D1,1)</f>
@@ -21094,11 +21087,11 @@
         <f t="shared" si="137"/>
         <v>,</v>
       </c>
-      <c r="P84" s="27" t="str">
+      <c r="P84" s="26" t="str">
         <f t="shared" si="137"/>
         <v>1</v>
       </c>
-      <c r="Q84" s="27" t="str">
+      <c r="Q84" s="26" t="str">
         <f t="shared" si="137"/>
         <v>3</v>
       </c>
@@ -21245,7 +21238,7 @@
         <v>0</v>
       </c>
       <c r="C85" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D85" s="18" t="str">
         <f>MID($C$85,D1,1)</f>
@@ -21295,23 +21288,23 @@
         <f t="shared" si="138"/>
         <v>,</v>
       </c>
-      <c r="P85" s="27" t="str">
+      <c r="P85" s="26" t="str">
         <f t="shared" si="138"/>
         <v>[</v>
       </c>
-      <c r="Q85" s="27" t="str">
+      <c r="Q85" s="26" t="str">
         <f t="shared" si="138"/>
         <v>6</v>
       </c>
-      <c r="R85" s="27" t="str">
+      <c r="R85" s="26" t="str">
         <f t="shared" si="138"/>
         <v>,</v>
       </c>
-      <c r="S85" s="27" t="str">
+      <c r="S85" s="26" t="str">
         <f t="shared" si="138"/>
         <v>7</v>
       </c>
-      <c r="T85" s="27" t="str">
+      <c r="T85" s="26" t="str">
         <f t="shared" si="138"/>
         <v>]</v>
       </c>
@@ -21446,7 +21439,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D86" s="18" t="str">
         <f>MID($C$86,D1,1)</f>
@@ -21552,11 +21545,11 @@
         <f t="shared" si="139"/>
         <v>,</v>
       </c>
-      <c r="AD86" s="27" t="str">
+      <c r="AD86" s="26" t="str">
         <f t="shared" si="139"/>
         <v>1</v>
       </c>
-      <c r="AE86" s="27" t="str">
+      <c r="AE86" s="26" t="str">
         <f t="shared" si="139"/>
         <v>0</v>
       </c>
@@ -21647,7 +21640,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D87" s="18" t="str">
         <f>MID($C$87,D1,1)</f>
@@ -21753,23 +21746,23 @@
         <f t="shared" si="140"/>
         <v>,</v>
       </c>
-      <c r="AD87" s="27" t="str">
+      <c r="AD87" s="26" t="str">
         <f t="shared" si="140"/>
         <v>[</v>
       </c>
-      <c r="AE87" s="27" t="str">
+      <c r="AE87" s="26" t="str">
         <f t="shared" si="140"/>
         <v>5</v>
       </c>
-      <c r="AF87" s="27" t="str">
+      <c r="AF87" s="26" t="str">
         <f t="shared" si="140"/>
         <v>,</v>
       </c>
-      <c r="AG87" s="27" t="str">
+      <c r="AG87" s="26" t="str">
         <f t="shared" si="140"/>
         <v>5</v>
       </c>
-      <c r="AH87" s="27" t="str">
+      <c r="AH87" s="26" t="str">
         <f t="shared" si="140"/>
         <v>]</v>
       </c>
@@ -21868,7 +21861,7 @@
         <v>0</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D88" s="18" t="str">
         <f>MID($C$88,D1,1)</f>
@@ -21966,11 +21959,11 @@
         <f t="shared" si="141"/>
         <v>[</v>
       </c>
-      <c r="AB88" s="27" t="str">
+      <c r="AB88" s="26" t="str">
         <f t="shared" si="141"/>
         <v>1</v>
       </c>
-      <c r="AC88" s="27" t="str">
+      <c r="AC88" s="26" t="str">
         <f t="shared" si="141"/>
         <v>4</v>
       </c>
@@ -22089,7 +22082,7 @@
         <v>0</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D89" s="18" t="str">
         <f>MID($C$89,D1,1)</f>
@@ -22187,23 +22180,23 @@
         <f t="shared" si="142"/>
         <v>[</v>
       </c>
-      <c r="AB89" s="27" t="str">
+      <c r="AB89" s="26" t="str">
         <f t="shared" si="142"/>
         <v>[</v>
       </c>
-      <c r="AC89" s="27" t="str">
+      <c r="AC89" s="26" t="str">
         <f t="shared" si="142"/>
         <v>7</v>
       </c>
-      <c r="AD89" s="27" t="str">
+      <c r="AD89" s="26" t="str">
         <f t="shared" si="142"/>
         <v>,</v>
       </c>
-      <c r="AE89" s="27" t="str">
+      <c r="AE89" s="26" t="str">
         <f t="shared" si="142"/>
         <v>7</v>
       </c>
-      <c r="AF89" s="27" t="str">
+      <c r="AF89" s="26" t="str">
         <f t="shared" si="142"/>
         <v>]</v>
       </c>
@@ -22310,7 +22303,7 @@
         <v>0</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D90" s="18" t="str">
         <f>MID($C$90,D1,1)</f>
@@ -22392,11 +22385,11 @@
         <f t="shared" si="143"/>
         <v>,</v>
       </c>
-      <c r="X90" s="27" t="str">
+      <c r="X90" s="26" t="str">
         <f t="shared" si="143"/>
         <v>1</v>
       </c>
-      <c r="Y90" s="27" t="str">
+      <c r="Y90" s="26" t="str">
         <f t="shared" si="143"/>
         <v>4</v>
       </c>
@@ -22531,7 +22524,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D91" s="18" t="str">
         <f>MID($C$91,D1,1)</f>
@@ -22613,23 +22606,23 @@
         <f t="shared" si="144"/>
         <v>,</v>
       </c>
-      <c r="X91" s="27" t="str">
+      <c r="X91" s="26" t="str">
         <f t="shared" si="144"/>
         <v>[</v>
       </c>
-      <c r="Y91" s="27" t="str">
+      <c r="Y91" s="26" t="str">
         <f t="shared" si="144"/>
         <v>7</v>
       </c>
-      <c r="Z91" s="27" t="str">
+      <c r="Z91" s="26" t="str">
         <f t="shared" si="144"/>
         <v>,</v>
       </c>
-      <c r="AA91" s="27" t="str">
+      <c r="AA91" s="26" t="str">
         <f t="shared" si="144"/>
         <v>7</v>
       </c>
-      <c r="AB91" s="27" t="str">
+      <c r="AB91" s="26" t="str">
         <f t="shared" si="144"/>
         <v>]</v>
       </c>
@@ -22752,7 +22745,7 @@
         <v>0</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D92" s="18" t="str">
         <f>MID($C$92,D1,1)</f>
@@ -22826,11 +22819,11 @@
         <f t="shared" si="145"/>
         <v>[</v>
       </c>
-      <c r="V92" s="27" t="str">
+      <c r="V92" s="26" t="str">
         <f t="shared" si="145"/>
         <v>1</v>
       </c>
-      <c r="W92" s="27" t="str">
+      <c r="W92" s="26" t="str">
         <f t="shared" si="145"/>
         <v>4</v>
       </c>
@@ -22973,7 +22966,7 @@
         <v>0</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D93" s="18" t="str">
         <f>MID($C$93,D1,1)</f>
@@ -23047,23 +23040,23 @@
         <f t="shared" si="146"/>
         <v>[</v>
       </c>
-      <c r="V93" s="27" t="str">
+      <c r="V93" s="26" t="str">
         <f t="shared" si="146"/>
         <v>[</v>
       </c>
-      <c r="W93" s="27" t="str">
+      <c r="W93" s="26" t="str">
         <f t="shared" si="146"/>
         <v>7</v>
       </c>
-      <c r="X93" s="27" t="str">
+      <c r="X93" s="26" t="str">
         <f t="shared" si="146"/>
         <v>,</v>
       </c>
-      <c r="Y93" s="27" t="str">
+      <c r="Y93" s="26" t="str">
         <f t="shared" si="146"/>
         <v>7</v>
       </c>
-      <c r="Z93" s="27" t="str">
+      <c r="Z93" s="26" t="str">
         <f t="shared" si="146"/>
         <v>]</v>
       </c>
@@ -23194,7 +23187,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D94" s="18" t="str">
         <f>MID($C$94,D1,1)</f>
@@ -23324,11 +23317,11 @@
         <f t="shared" si="147"/>
         <v>[</v>
       </c>
-      <c r="AJ94" s="27" t="str">
+      <c r="AJ94" s="26" t="str">
         <f t="shared" si="147"/>
         <v>2</v>
       </c>
-      <c r="AK94" s="27" t="str">
+      <c r="AK94" s="26" t="str">
         <f t="shared" si="147"/>
         <v>1</v>
       </c>
@@ -23415,7 +23408,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D95" s="18" t="str">
         <f>MID($C$95,D1,1)</f>
@@ -23549,11 +23542,11 @@
         <f t="shared" si="148"/>
         <v>[</v>
       </c>
-      <c r="AK95" s="27" t="str">
+      <c r="AK95" s="26" t="str">
         <f t="shared" si="148"/>
         <v>1</v>
       </c>
-      <c r="AL95" s="27" t="str">
+      <c r="AL95" s="26" t="str">
         <f t="shared" si="148"/>
         <v>0</v>
       </c>
@@ -23636,197 +23629,197 @@
         <v>0</v>
       </c>
       <c r="C96" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="D96" s="24" t="str">
+        <v>167</v>
+      </c>
+      <c r="D96" s="23" t="str">
         <f>MID($C$96,D1,1)</f>
         <v>[</v>
       </c>
-      <c r="E96" s="24" t="str">
+      <c r="E96" s="23" t="str">
         <f t="shared" ref="E96:BC96" si="149">MID($C$96,E1,1)</f>
         <v>[</v>
       </c>
-      <c r="F96" s="24" t="str">
+      <c r="F96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="G96" s="24" t="str">
+      <c r="G96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="H96" s="24" t="str">
+      <c r="H96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>6</v>
       </c>
-      <c r="I96" s="24" t="str">
+      <c r="I96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="J96" s="24" t="str">
+      <c r="J96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>6</v>
       </c>
-      <c r="K96" s="24" t="str">
+      <c r="K96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="L96" s="24" t="str">
+      <c r="L96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="M96" s="24" t="str">
+      <c r="M96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="N96" s="24" t="str">
+      <c r="N96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>6</v>
       </c>
-      <c r="O96" s="24" t="str">
+      <c r="O96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="P96" s="24" t="str">
+      <c r="P96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>7</v>
       </c>
-      <c r="Q96" s="24" t="str">
+      <c r="Q96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="R96" s="24" t="str">
+      <c r="R96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="S96" s="24" t="str">
+      <c r="S96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="T96" s="24" t="str">
+      <c r="T96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="U96" s="24" t="str">
+      <c r="U96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="V96" s="24" t="str">
+      <c r="V96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>0</v>
       </c>
-      <c r="W96" s="24" t="str">
+      <c r="W96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="X96" s="24" t="str">
+      <c r="X96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>7</v>
       </c>
-      <c r="Y96" s="24" t="str">
+      <c r="Y96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="Z96" s="24" t="str">
+      <c r="Z96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="AA96" s="24" t="str">
+      <c r="AA96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="AB96" s="24" t="str">
+      <c r="AB96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>7</v>
       </c>
-      <c r="AC96" s="24" t="str">
+      <c r="AC96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="AD96" s="24" t="str">
+      <c r="AD96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>7</v>
       </c>
-      <c r="AE96" s="24" t="str">
+      <c r="AE96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="AF96" s="24" t="str">
+      <c r="AF96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="AG96" s="24" t="str">
+      <c r="AG96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="AH96" s="24" t="str">
+      <c r="AH96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="AI96" s="24" t="str">
+      <c r="AI96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="AJ96" s="24" t="str">
+      <c r="AJ96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="AK96" s="24" t="str">
+      <c r="AK96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>[</v>
       </c>
-      <c r="AL96" s="24" t="str">
+      <c r="AL96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>5</v>
       </c>
-      <c r="AM96" s="24" t="str">
+      <c r="AM96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="AN96" s="24" t="str">
+      <c r="AN96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>5</v>
       </c>
-      <c r="AO96" s="24" t="str">
+      <c r="AO96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="AP96" s="24" t="str">
+      <c r="AP96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="AQ96" s="28" t="str">
+      <c r="AQ96" s="27" t="str">
         <f t="shared" si="149"/>
         <v>1</v>
       </c>
-      <c r="AR96" s="28" t="str">
+      <c r="AR96" s="27" t="str">
         <f t="shared" si="149"/>
         <v>1</v>
       </c>
-      <c r="AS96" s="24" t="str">
+      <c r="AS96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="AT96" s="24" t="str">
+      <c r="AT96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>,</v>
       </c>
-      <c r="AU96" s="24" t="str">
+      <c r="AU96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>9</v>
       </c>
-      <c r="AV96" s="24" t="str">
+      <c r="AV96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="AW96" s="24" t="str">
+      <c r="AW96" s="23" t="str">
         <f t="shared" si="149"/>
         <v>]</v>
       </c>
-      <c r="AX96" s="24" t="str">
+      <c r="AX96" s="23" t="str">
         <f t="shared" si="149"/>
         <v/>
       </c>
-      <c r="AY96" s="24" t="str">
+      <c r="AY96" s="23" t="str">
         <f t="shared" si="149"/>
         <v/>
       </c>
@@ -23857,197 +23850,197 @@
         <v>0</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>170</v>
-      </c>
-      <c r="D97" s="24" t="str">
+        <v>168</v>
+      </c>
+      <c r="D97" s="23" t="str">
         <f>MID($C$97,D1,1)</f>
         <v>[</v>
       </c>
-      <c r="E97" s="24" t="str">
+      <c r="E97" s="23" t="str">
         <f t="shared" ref="E97:BC97" si="150">MID($C$97,E1,1)</f>
         <v>[</v>
       </c>
-      <c r="F97" s="24" t="str">
+      <c r="F97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="G97" s="24" t="str">
+      <c r="G97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="H97" s="24" t="str">
+      <c r="H97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>6</v>
       </c>
-      <c r="I97" s="24" t="str">
+      <c r="I97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="J97" s="24" t="str">
+      <c r="J97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>6</v>
       </c>
-      <c r="K97" s="24" t="str">
+      <c r="K97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="L97" s="24" t="str">
+      <c r="L97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="M97" s="24" t="str">
+      <c r="M97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="N97" s="29" t="str">
+      <c r="N97" s="28" t="str">
         <f t="shared" si="150"/>
         <v>6</v>
       </c>
-      <c r="O97" s="24" t="str">
+      <c r="O97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="P97" s="24" t="str">
+      <c r="P97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>7</v>
       </c>
-      <c r="Q97" s="24" t="str">
+      <c r="Q97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="R97" s="24" t="str">
+      <c r="R97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="S97" s="24" t="str">
+      <c r="S97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="T97" s="24" t="str">
+      <c r="T97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="U97" s="24" t="str">
+      <c r="U97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="V97" s="24" t="str">
+      <c r="V97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>0</v>
       </c>
-      <c r="W97" s="24" t="str">
+      <c r="W97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="X97" s="24" t="str">
+      <c r="X97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>7</v>
       </c>
-      <c r="Y97" s="24" t="str">
+      <c r="Y97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="Z97" s="24" t="str">
+      <c r="Z97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="AA97" s="24" t="str">
+      <c r="AA97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="AB97" s="24" t="str">
+      <c r="AB97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>7</v>
       </c>
-      <c r="AC97" s="24" t="str">
+      <c r="AC97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="AD97" s="24" t="str">
+      <c r="AD97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>7</v>
       </c>
-      <c r="AE97" s="24" t="str">
+      <c r="AE97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="AF97" s="24" t="str">
+      <c r="AF97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="AG97" s="24" t="str">
+      <c r="AG97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="AH97" s="24" t="str">
+      <c r="AH97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="AI97" s="24" t="str">
+      <c r="AI97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="AJ97" s="24" t="str">
+      <c r="AJ97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="AK97" s="24" t="str">
+      <c r="AK97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="AL97" s="24" t="str">
+      <c r="AL97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>5</v>
       </c>
-      <c r="AM97" s="24" t="str">
+      <c r="AM97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="AN97" s="24" t="str">
+      <c r="AN97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>5</v>
       </c>
-      <c r="AO97" s="24" t="str">
+      <c r="AO97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="AP97" s="24" t="str">
+      <c r="AP97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="AQ97" s="24" t="str">
+      <c r="AQ97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>[</v>
       </c>
-      <c r="AR97" s="24" t="str">
+      <c r="AR97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>5</v>
       </c>
-      <c r="AS97" s="24" t="str">
+      <c r="AS97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="AT97" s="24" t="str">
+      <c r="AT97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>6</v>
       </c>
-      <c r="AU97" s="24" t="str">
+      <c r="AU97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="AV97" s="24" t="str">
+      <c r="AV97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>
-      <c r="AW97" s="24" t="str">
+      <c r="AW97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>,</v>
       </c>
-      <c r="AX97" s="24" t="str">
+      <c r="AX97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>9</v>
       </c>
-      <c r="AY97" s="24" t="str">
+      <c r="AY97" s="23" t="str">
         <f t="shared" si="150"/>
         <v>]</v>
       </c>

</xml_diff>